<commit_message>
Update .gitignore, style.css, and xbee_data files, actual_xbee_list
</commit_message>
<xml_diff>
--- a/misc/component_dev.xlsx
+++ b/misc/component_dev.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kunjs\Desktop\Cansat\SEM 7\DEV\GUI\CANSAT_data_viz\with_dash\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB76398F-6821-4D43-893A-5C1BD8464A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81198D0-16DE-4FD5-9CA6-2B0D566C899D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2771C4AE-BC75-4925-8982-CB62CB8CB148}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2771C4AE-BC75-4925-8982-CB62CB8CB148}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1056E77F-D55F-4E00-AFBA-4953BF33AC2A}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA8D553-C64A-40C4-A239-79370E1413E6}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>